<commit_message>
fix transcription errors in phono reps of some wordsets
</commit_message>
<xml_diff>
--- a/inst/extdata/g1979a1.xlsx
+++ b/inst/extdata/g1979a1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage.yale.edu\home\HASKINS_A195-997121-haskinslab\07 - Modeling\wordsets for model criticism\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\braze\R\development\FDBwordsets-dev\FDBwordsets\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" tabRatio="500"/>
+    <workbookView xWindow="1308" yWindow="0" windowWidth="20604" windowHeight="8484" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="343">
   <si>
     <t>Glushko-1979-Appendix-1</t>
   </si>
@@ -1043,12 +1043,24 @@
   </si>
   <si>
     <t>sUl</t>
+  </si>
+  <si>
+    <t>k@T</t>
+  </si>
+  <si>
+    <t>kaT</t>
+  </si>
+  <si>
+    <t>kob</t>
+  </si>
+  <si>
+    <t>koz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1370,21 +1382,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I134" sqref="I134"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.125"/>
+    <col min="1" max="1025" width="8.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1424,7 +1436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1444,7 +1456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>339</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -1464,7 +1476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -1484,7 +1496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1504,7 +1516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1544,7 +1556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1584,7 +1596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1604,7 +1616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1624,7 +1636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1664,7 +1676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1704,7 +1716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1724,7 +1736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1744,7 +1756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1784,7 +1796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1804,7 +1816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1824,7 +1836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1844,7 +1856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1864,7 +1876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1884,7 +1896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1904,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1924,7 +1936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1944,7 +1956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1964,7 +1976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1984,7 +1996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8</v>
       </c>
@@ -2004,7 +2016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
@@ -2024,7 +2036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8</v>
       </c>
@@ -2044,7 +2056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9</v>
       </c>
@@ -2064,7 +2076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>9</v>
       </c>
@@ -2084,7 +2096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9</v>
       </c>
@@ -2104,7 +2116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>9</v>
       </c>
@@ -2124,7 +2136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10</v>
       </c>
@@ -2144,7 +2156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10</v>
       </c>
@@ -2164,7 +2176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10</v>
       </c>
@@ -2184,7 +2196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
@@ -2204,7 +2216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
@@ -2224,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>11</v>
       </c>
@@ -2244,7 +2256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>11</v>
       </c>
@@ -2264,7 +2276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>11</v>
       </c>
@@ -2284,7 +2296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>12</v>
       </c>
@@ -2304,7 +2316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>12</v>
       </c>
@@ -2324,7 +2336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>12</v>
       </c>
@@ -2344,7 +2356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>12</v>
       </c>
@@ -2364,7 +2376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>13</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>13</v>
       </c>
@@ -2404,7 +2416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>13</v>
       </c>
@@ -2424,7 +2436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>13</v>
       </c>
@@ -2444,7 +2456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>14</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>14</v>
       </c>
@@ -2484,7 +2496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14</v>
       </c>
@@ -2504,7 +2516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>14</v>
       </c>
@@ -2524,7 +2536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>15</v>
       </c>
@@ -2544,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -2564,7 +2576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -2584,7 +2596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
@@ -2604,7 +2616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>16</v>
       </c>
@@ -2624,7 +2636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>16</v>
       </c>
@@ -2644,7 +2656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>16</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>16</v>
       </c>
@@ -2684,7 +2696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>17</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>17</v>
       </c>
@@ -2724,7 +2736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>17</v>
       </c>
@@ -2744,7 +2756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>17</v>
       </c>
@@ -2764,7 +2776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>18</v>
       </c>
@@ -2784,7 +2796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>18</v>
       </c>
@@ -2804,7 +2816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>18</v>
       </c>
@@ -2824,7 +2836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>18</v>
       </c>
@@ -2844,7 +2856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>19</v>
       </c>
@@ -2864,7 +2876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>19</v>
       </c>
@@ -2884,7 +2896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>19</v>
       </c>
@@ -2904,7 +2916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>19</v>
       </c>
@@ -2924,7 +2936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>20</v>
       </c>
@@ -2944,7 +2956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>20</v>
       </c>
@@ -2964,7 +2976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -2972,7 +2984,7 @@
         <v>149</v>
       </c>
       <c r="C81" t="s">
-        <v>150</v>
+        <v>341</v>
       </c>
       <c r="D81" t="s">
         <v>16</v>
@@ -2984,7 +2996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>20</v>
       </c>
@@ -2992,7 +3004,7 @@
         <v>151</v>
       </c>
       <c r="C82" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="D82" t="s">
         <v>16</v>
@@ -3004,7 +3016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>21</v>
       </c>
@@ -3024,7 +3036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>21</v>
       </c>
@@ -3044,7 +3056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>21</v>
       </c>
@@ -3064,7 +3076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>21</v>
       </c>
@@ -3084,7 +3096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>22</v>
       </c>
@@ -3104,7 +3116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>22</v>
       </c>
@@ -3124,7 +3136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>22</v>
       </c>
@@ -3144,7 +3156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>22</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>23</v>
       </c>
@@ -3184,7 +3196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>23</v>
       </c>
@@ -3204,7 +3216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>23</v>
       </c>
@@ -3224,7 +3236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>23</v>
       </c>
@@ -3244,7 +3256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>24</v>
       </c>
@@ -3264,7 +3276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>24</v>
       </c>
@@ -3284,7 +3296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>24</v>
       </c>
@@ -3304,7 +3316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>24</v>
       </c>
@@ -3324,7 +3336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>25</v>
       </c>
@@ -3344,7 +3356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>25</v>
       </c>
@@ -3364,7 +3376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>25</v>
       </c>
@@ -3384,7 +3396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>25</v>
       </c>
@@ -3404,7 +3416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>26</v>
       </c>
@@ -3424,7 +3436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>26</v>
       </c>
@@ -3444,7 +3456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>26</v>
       </c>
@@ -3464,7 +3476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>26</v>
       </c>
@@ -3484,7 +3496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>27</v>
       </c>
@@ -3504,7 +3516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>27</v>
       </c>
@@ -3524,7 +3536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>27</v>
       </c>
@@ -3544,7 +3556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>27</v>
       </c>
@@ -3564,7 +3576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>28</v>
       </c>
@@ -3584,7 +3596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>28</v>
       </c>
@@ -3604,7 +3616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>28</v>
       </c>
@@ -3624,7 +3636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>28</v>
       </c>
@@ -3644,7 +3656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>29</v>
       </c>
@@ -3664,7 +3676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>29</v>
       </c>
@@ -3684,7 +3696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>29</v>
       </c>
@@ -3704,7 +3716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>29</v>
       </c>
@@ -3724,7 +3736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>30</v>
       </c>
@@ -3744,7 +3756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>30</v>
       </c>
@@ -3764,7 +3776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>30</v>
       </c>
@@ -3784,7 +3796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>30</v>
       </c>
@@ -3804,7 +3816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>31</v>
       </c>
@@ -3824,7 +3836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>31</v>
       </c>
@@ -3844,7 +3856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>31</v>
       </c>
@@ -3864,7 +3876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>31</v>
       </c>
@@ -3884,7 +3896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>32</v>
       </c>
@@ -3904,7 +3916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>32</v>
       </c>
@@ -3924,7 +3936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>32</v>
       </c>
@@ -3944,7 +3956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>32</v>
       </c>
@@ -3964,7 +3976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>33</v>
       </c>
@@ -3984,7 +3996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>33</v>
       </c>
@@ -4004,7 +4016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>33</v>
       </c>
@@ -4024,7 +4036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>33</v>
       </c>
@@ -4044,7 +4056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>34</v>
       </c>
@@ -4064,7 +4076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>34</v>
       </c>
@@ -4084,7 +4096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>34</v>
       </c>
@@ -4104,7 +4116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>34</v>
       </c>
@@ -4124,7 +4136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>35</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>35</v>
       </c>
@@ -4164,7 +4176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>35</v>
       </c>
@@ -4184,7 +4196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>35</v>
       </c>
@@ -4204,7 +4216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>36</v>
       </c>
@@ -4224,7 +4236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>36</v>
       </c>
@@ -4244,7 +4256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>36</v>
       </c>
@@ -4264,7 +4276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>36</v>
       </c>
@@ -4284,7 +4296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>37</v>
       </c>
@@ -4304,7 +4316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>37</v>
       </c>
@@ -4324,7 +4336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>37</v>
       </c>
@@ -4344,7 +4356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>37</v>
       </c>
@@ -4364,7 +4376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>38</v>
       </c>
@@ -4384,7 +4396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>38</v>
       </c>
@@ -4404,7 +4416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>38</v>
       </c>
@@ -4424,7 +4436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>38</v>
       </c>
@@ -4444,7 +4456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>39</v>
       </c>
@@ -4464,7 +4476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>39</v>
       </c>
@@ -4484,7 +4496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>39</v>
       </c>
@@ -4504,7 +4516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>39</v>
       </c>
@@ -4524,7 +4536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>40</v>
       </c>
@@ -4544,7 +4556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>40</v>
       </c>
@@ -4564,7 +4576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>40</v>
       </c>
@@ -4584,7 +4596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>40</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>41</v>
       </c>
@@ -4624,7 +4636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>41</v>
       </c>
@@ -4644,7 +4656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>41</v>
       </c>
@@ -4664,7 +4676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>41</v>
       </c>
@@ -4684,7 +4696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>42</v>
       </c>
@@ -4704,7 +4716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>42</v>
       </c>
@@ -4724,7 +4736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>42</v>
       </c>
@@ -4744,7 +4756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>42</v>
       </c>
@@ -4764,7 +4776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>43</v>
       </c>
@@ -4784,7 +4796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>43</v>
       </c>
@@ -4804,7 +4816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>43</v>
       </c>
@@ -4824,7 +4836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>43</v>
       </c>
@@ -4858,17 +4870,17 @@
       <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.125"/>
+    <col min="1" max="1025" width="8.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4888,7 +4900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4908,7 +4920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4928,7 +4940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4948,7 +4960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4968,7 +4980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4988,7 +5000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -5008,7 +5020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -5028,7 +5040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -5048,7 +5060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5068,7 +5080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -5088,7 +5100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -5108,7 +5120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -5128,7 +5140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -5148,7 +5160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -5168,7 +5180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -5188,7 +5200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -5208,7 +5220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -5228,7 +5240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5248,7 +5260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -5268,7 +5280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -5288,7 +5300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -5308,7 +5320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -5328,7 +5340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -5348,7 +5360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -5368,7 +5380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -5388,7 +5400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7</v>
       </c>
@@ -5408,7 +5420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -5428,7 +5440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7</v>
       </c>
@@ -5448,7 +5460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -5468,7 +5480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8</v>
       </c>
@@ -5488,7 +5500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
@@ -5508,7 +5520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8</v>
       </c>
@@ -5528,7 +5540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9</v>
       </c>
@@ -5548,7 +5560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>9</v>
       </c>
@@ -5568,7 +5580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9</v>
       </c>
@@ -5588,7 +5600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>9</v>
       </c>
@@ -5608,7 +5620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10</v>
       </c>
@@ -5628,7 +5640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10</v>
       </c>
@@ -5648,7 +5660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10</v>
       </c>
@@ -5668,7 +5680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
@@ -5688,7 +5700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
@@ -5708,7 +5720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>11</v>
       </c>
@@ -5728,7 +5740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>11</v>
       </c>
@@ -5748,7 +5760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>11</v>
       </c>
@@ -5768,7 +5780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>12</v>
       </c>
@@ -5788,7 +5800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>12</v>
       </c>
@@ -5808,7 +5820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>12</v>
       </c>
@@ -5828,7 +5840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>12</v>
       </c>
@@ -5848,7 +5860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>13</v>
       </c>
@@ -5868,7 +5880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>13</v>
       </c>
@@ -5888,7 +5900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>13</v>
       </c>
@@ -5908,7 +5920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>13</v>
       </c>
@@ -5928,7 +5940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>14</v>
       </c>
@@ -5948,7 +5960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>14</v>
       </c>
@@ -5968,7 +5980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14</v>
       </c>
@@ -5988,7 +6000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>14</v>
       </c>
@@ -6008,7 +6020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>15</v>
       </c>
@@ -6028,7 +6040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -6048,7 +6060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -6068,7 +6080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
@@ -6088,7 +6100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>16</v>
       </c>
@@ -6108,7 +6120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>16</v>
       </c>
@@ -6128,7 +6140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>16</v>
       </c>
@@ -6148,7 +6160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>16</v>
       </c>
@@ -6168,7 +6180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>17</v>
       </c>
@@ -6188,7 +6200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>17</v>
       </c>
@@ -6208,7 +6220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>17</v>
       </c>
@@ -6228,7 +6240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>17</v>
       </c>
@@ -6248,7 +6260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>18</v>
       </c>
@@ -6268,7 +6280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>18</v>
       </c>
@@ -6288,7 +6300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>18</v>
       </c>
@@ -6308,7 +6320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>18</v>
       </c>
@@ -6328,7 +6340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>19</v>
       </c>
@@ -6348,7 +6360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>19</v>
       </c>
@@ -6368,7 +6380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>19</v>
       </c>
@@ -6388,7 +6400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>19</v>
       </c>
@@ -6408,7 +6420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>20</v>
       </c>
@@ -6428,7 +6440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>20</v>
       </c>
@@ -6448,7 +6460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -6468,7 +6480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>20</v>
       </c>
@@ -6488,7 +6500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>21</v>
       </c>
@@ -6508,7 +6520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>21</v>
       </c>
@@ -6528,7 +6540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>21</v>
       </c>
@@ -6548,7 +6560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>21</v>
       </c>
@@ -6568,7 +6580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>22</v>
       </c>
@@ -6588,7 +6600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>22</v>
       </c>
@@ -6608,7 +6620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>22</v>
       </c>
@@ -6628,7 +6640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>22</v>
       </c>
@@ -6648,7 +6660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>23</v>
       </c>
@@ -6668,7 +6680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>23</v>
       </c>
@@ -6688,7 +6700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>23</v>
       </c>
@@ -6708,7 +6720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>23</v>
       </c>
@@ -6728,7 +6740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>24</v>
       </c>
@@ -6748,7 +6760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>24</v>
       </c>
@@ -6768,7 +6780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>24</v>
       </c>
@@ -6788,7 +6800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>24</v>
       </c>
@@ -6808,7 +6820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>25</v>
       </c>
@@ -6828,7 +6840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>25</v>
       </c>
@@ -6848,7 +6860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>25</v>
       </c>
@@ -6868,7 +6880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>25</v>
       </c>
@@ -6888,7 +6900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>26</v>
       </c>
@@ -6908,7 +6920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>26</v>
       </c>
@@ -6928,7 +6940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>26</v>
       </c>
@@ -6948,7 +6960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>26</v>
       </c>
@@ -6968,7 +6980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>27</v>
       </c>
@@ -6988,7 +7000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>27</v>
       </c>
@@ -7008,7 +7020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>27</v>
       </c>
@@ -7028,7 +7040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>27</v>
       </c>
@@ -7048,7 +7060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>28</v>
       </c>
@@ -7068,7 +7080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>28</v>
       </c>
@@ -7088,7 +7100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>28</v>
       </c>
@@ -7108,7 +7120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>28</v>
       </c>
@@ -7128,7 +7140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>29</v>
       </c>
@@ -7148,7 +7160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>29</v>
       </c>
@@ -7168,7 +7180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>29</v>
       </c>
@@ -7188,7 +7200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>29</v>
       </c>
@@ -7208,7 +7220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>30</v>
       </c>
@@ -7228,7 +7240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>30</v>
       </c>
@@ -7248,7 +7260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>30</v>
       </c>
@@ -7268,7 +7280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>30</v>
       </c>
@@ -7288,7 +7300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>31</v>
       </c>
@@ -7308,7 +7320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>31</v>
       </c>
@@ -7328,7 +7340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>31</v>
       </c>
@@ -7348,7 +7360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>31</v>
       </c>
@@ -7368,7 +7380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>32</v>
       </c>
@@ -7388,7 +7400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>32</v>
       </c>
@@ -7408,7 +7420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>32</v>
       </c>
@@ -7428,7 +7440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>32</v>
       </c>
@@ -7448,7 +7460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>33</v>
       </c>
@@ -7468,7 +7480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>33</v>
       </c>
@@ -7488,7 +7500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>33</v>
       </c>
@@ -7508,7 +7520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>33</v>
       </c>
@@ -7528,7 +7540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>34</v>
       </c>
@@ -7548,7 +7560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>34</v>
       </c>
@@ -7568,7 +7580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>34</v>
       </c>
@@ -7588,7 +7600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>34</v>
       </c>
@@ -7608,7 +7620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>35</v>
       </c>
@@ -7628,7 +7640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>35</v>
       </c>
@@ -7648,7 +7660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>35</v>
       </c>
@@ -7668,7 +7680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>35</v>
       </c>
@@ -7688,7 +7700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>36</v>
       </c>
@@ -7708,7 +7720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>36</v>
       </c>
@@ -7728,7 +7740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>36</v>
       </c>
@@ -7748,7 +7760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>36</v>
       </c>
@@ -7768,7 +7780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>37</v>
       </c>
@@ -7788,7 +7800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>37</v>
       </c>
@@ -7808,7 +7820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>37</v>
       </c>
@@ -7828,7 +7840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>37</v>
       </c>
@@ -7848,7 +7860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>38</v>
       </c>
@@ -7868,7 +7880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>38</v>
       </c>
@@ -7888,7 +7900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>38</v>
       </c>
@@ -7908,7 +7920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>38</v>
       </c>
@@ -7928,7 +7940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>39</v>
       </c>
@@ -7948,7 +7960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>39</v>
       </c>
@@ -7968,7 +7980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>39</v>
       </c>
@@ -7988,7 +8000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>39</v>
       </c>
@@ -8008,7 +8020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>40</v>
       </c>
@@ -8028,7 +8040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>40</v>
       </c>
@@ -8048,7 +8060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>40</v>
       </c>
@@ -8068,7 +8080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>40</v>
       </c>
@@ -8088,7 +8100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>41</v>
       </c>
@@ -8108,7 +8120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>41</v>
       </c>
@@ -8128,7 +8140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>41</v>
       </c>
@@ -8148,7 +8160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>41</v>
       </c>
@@ -8168,7 +8180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>42</v>
       </c>
@@ -8188,7 +8200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>42</v>
       </c>
@@ -8208,7 +8220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>42</v>
       </c>
@@ -8228,7 +8240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>42</v>
       </c>
@@ -8248,7 +8260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>43</v>
       </c>
@@ -8268,7 +8280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>43</v>
       </c>
@@ -8288,7 +8300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>43</v>
       </c>
@@ -8308,7 +8320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>43</v>
       </c>
@@ -8342,18 +8354,18 @@
       <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.125"/>
+    <col min="1" max="1025" width="8.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>IF(Sheet1!A1=Sheet2!A1,Sheet1!A1,"")</f>
         <v>Glushko-1979-Appendix-1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(Sheet1!A2=Sheet2!A2,Sheet1!A2,"")</f>
         <v>set</v>
@@ -8379,7 +8391,7 @@
         <v>regularity</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(Sheet1!A3=Sheet2!A3,Sheet1!A3,"")</f>
         <v>1</v>
@@ -8405,7 +8417,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>IF(Sheet1!A4=Sheet2!A4,Sheet1!A4,"")</f>
         <v>1</v>
@@ -8431,7 +8443,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>IF(Sheet1!A5=Sheet2!A5,Sheet1!A5,"")</f>
         <v>1</v>
@@ -8442,7 +8454,7 @@
       </c>
       <c r="C5" t="str">
         <f>IF(Sheet1!C5=Sheet2!C5,Sheet1!C5,"")</f>
-        <v>c@T</v>
+        <v/>
       </c>
       <c r="D5" t="str">
         <f>IF(Sheet1!D5=Sheet2!D5,Sheet1!D5,"")</f>
@@ -8457,7 +8469,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>IF(Sheet1!A6=Sheet2!A6,Sheet1!A6,"")</f>
         <v>1</v>
@@ -8468,7 +8480,7 @@
       </c>
       <c r="C6" t="str">
         <f>IF(Sheet1!C6=Sheet2!C6,Sheet1!C6,"")</f>
-        <v>caT</v>
+        <v/>
       </c>
       <c r="D6" t="str">
         <f>IF(Sheet1!D6=Sheet2!D6,Sheet1!D6,"")</f>
@@ -8483,7 +8495,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>IF(Sheet1!A7=Sheet2!A7,Sheet1!A7,"")</f>
         <v>2</v>
@@ -8509,7 +8521,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>IF(Sheet1!A8=Sheet2!A8,Sheet1!A8,"")</f>
         <v>2</v>
@@ -8535,7 +8547,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>IF(Sheet1!A9=Sheet2!A9,Sheet1!A9,"")</f>
         <v>2</v>
@@ -8561,7 +8573,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>IF(Sheet1!A10=Sheet2!A10,Sheet1!A10,"")</f>
         <v>2</v>
@@ -8587,7 +8599,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>IF(Sheet1!A11=Sheet2!A11,Sheet1!A11,"")</f>
         <v>3</v>
@@ -8613,7 +8625,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>IF(Sheet1!A12=Sheet2!A12,Sheet1!A12,"")</f>
         <v>3</v>
@@ -8639,7 +8651,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>IF(Sheet1!A13=Sheet2!A13,Sheet1!A13,"")</f>
         <v>3</v>
@@ -8665,7 +8677,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>IF(Sheet1!A14=Sheet2!A14,Sheet1!A14,"")</f>
         <v>3</v>
@@ -8691,7 +8703,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>IF(Sheet1!A15=Sheet2!A15,Sheet1!A15,"")</f>
         <v>4</v>
@@ -8717,7 +8729,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>IF(Sheet1!A16=Sheet2!A16,Sheet1!A16,"")</f>
         <v>4</v>
@@ -8743,7 +8755,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>IF(Sheet1!A17=Sheet2!A17,Sheet1!A17,"")</f>
         <v>4</v>
@@ -8769,7 +8781,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>IF(Sheet1!A18=Sheet2!A18,Sheet1!A18,"")</f>
         <v>4</v>
@@ -8795,7 +8807,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <f>IF(Sheet1!A19=Sheet2!A19,Sheet1!A19,"")</f>
         <v>5</v>
@@ -8821,7 +8833,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <f>IF(Sheet1!A20=Sheet2!A20,Sheet1!A20,"")</f>
         <v>5</v>
@@ -8847,7 +8859,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <f>IF(Sheet1!A21=Sheet2!A21,Sheet1!A21,"")</f>
         <v>5</v>
@@ -8873,7 +8885,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>IF(Sheet1!A22=Sheet2!A22,Sheet1!A22,"")</f>
         <v>5</v>
@@ -8899,7 +8911,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>IF(Sheet1!A23=Sheet2!A23,Sheet1!A23,"")</f>
         <v>6</v>
@@ -8925,7 +8937,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>IF(Sheet1!A24=Sheet2!A24,Sheet1!A24,"")</f>
         <v>6</v>
@@ -8951,7 +8963,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <f>IF(Sheet1!A25=Sheet2!A25,Sheet1!A25,"")</f>
         <v>6</v>
@@ -8977,7 +8989,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>IF(Sheet1!A26=Sheet2!A26,Sheet1!A26,"")</f>
         <v>6</v>
@@ -9003,7 +9015,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>IF(Sheet1!A27=Sheet2!A27,Sheet1!A27,"")</f>
         <v>7</v>
@@ -9029,7 +9041,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>IF(Sheet1!A28=Sheet2!A28,Sheet1!A28,"")</f>
         <v>7</v>
@@ -9055,7 +9067,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>IF(Sheet1!A29=Sheet2!A29,Sheet1!A29,"")</f>
         <v>7</v>
@@ -9081,7 +9093,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <f>IF(Sheet1!A30=Sheet2!A30,Sheet1!A30,"")</f>
         <v>7</v>
@@ -9107,7 +9119,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>IF(Sheet1!A31=Sheet2!A31,Sheet1!A31,"")</f>
         <v>8</v>
@@ -9133,7 +9145,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>IF(Sheet1!A32=Sheet2!A32,Sheet1!A32,"")</f>
         <v>8</v>
@@ -9159,7 +9171,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <f>IF(Sheet1!A33=Sheet2!A33,Sheet1!A33,"")</f>
         <v>8</v>
@@ -9185,7 +9197,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>IF(Sheet1!A34=Sheet2!A34,Sheet1!A34,"")</f>
         <v>8</v>
@@ -9211,7 +9223,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>IF(Sheet1!A35=Sheet2!A35,Sheet1!A35,"")</f>
         <v>9</v>
@@ -9237,7 +9249,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>IF(Sheet1!A36=Sheet2!A36,Sheet1!A36,"")</f>
         <v>9</v>
@@ -9263,7 +9275,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>IF(Sheet1!A37=Sheet2!A37,Sheet1!A37,"")</f>
         <v>9</v>
@@ -9289,7 +9301,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>IF(Sheet1!A38=Sheet2!A38,Sheet1!A38,"")</f>
         <v>9</v>
@@ -9315,7 +9327,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>IF(Sheet1!A39=Sheet2!A39,Sheet1!A39,"")</f>
         <v>10</v>
@@ -9341,7 +9353,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>IF(Sheet1!A40=Sheet2!A40,Sheet1!A40,"")</f>
         <v>10</v>
@@ -9367,7 +9379,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>IF(Sheet1!A41=Sheet2!A41,Sheet1!A41,"")</f>
         <v>10</v>
@@ -9393,7 +9405,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <f>IF(Sheet1!A42=Sheet2!A42,Sheet1!A42,"")</f>
         <v>10</v>
@@ -9419,7 +9431,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <f>IF(Sheet1!A43=Sheet2!A43,Sheet1!A43,"")</f>
         <v>11</v>
@@ -9445,7 +9457,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <f>IF(Sheet1!A44=Sheet2!A44,Sheet1!A44,"")</f>
         <v>11</v>
@@ -9471,7 +9483,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <f>IF(Sheet1!A45=Sheet2!A45,Sheet1!A45,"")</f>
         <v>11</v>
@@ -9497,7 +9509,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <f>IF(Sheet1!A46=Sheet2!A46,Sheet1!A46,"")</f>
         <v>11</v>
@@ -9523,7 +9535,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <f>IF(Sheet1!A47=Sheet2!A47,Sheet1!A47,"")</f>
         <v>12</v>
@@ -9549,7 +9561,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <f>IF(Sheet1!A48=Sheet2!A48,Sheet1!A48,"")</f>
         <v>12</v>
@@ -9575,7 +9587,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <f>IF(Sheet1!A49=Sheet2!A49,Sheet1!A49,"")</f>
         <v>12</v>
@@ -9601,7 +9613,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <f>IF(Sheet1!A50=Sheet2!A50,Sheet1!A50,"")</f>
         <v>12</v>
@@ -9627,7 +9639,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <f>IF(Sheet1!A51=Sheet2!A51,Sheet1!A51,"")</f>
         <v>13</v>
@@ -9653,7 +9665,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <f>IF(Sheet1!A52=Sheet2!A52,Sheet1!A52,"")</f>
         <v>13</v>
@@ -9679,7 +9691,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <f>IF(Sheet1!A53=Sheet2!A53,Sheet1!A53,"")</f>
         <v>13</v>
@@ -9705,7 +9717,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <f>IF(Sheet1!A54=Sheet2!A54,Sheet1!A54,"")</f>
         <v>13</v>
@@ -9731,7 +9743,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <f>IF(Sheet1!A55=Sheet2!A55,Sheet1!A55,"")</f>
         <v>14</v>
@@ -9757,7 +9769,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <f>IF(Sheet1!A56=Sheet2!A56,Sheet1!A56,"")</f>
         <v>14</v>
@@ -9783,7 +9795,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <f>IF(Sheet1!A57=Sheet2!A57,Sheet1!A57,"")</f>
         <v>14</v>
@@ -9809,7 +9821,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <f>IF(Sheet1!A58=Sheet2!A58,Sheet1!A58,"")</f>
         <v>14</v>
@@ -9835,7 +9847,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <f>IF(Sheet1!A59=Sheet2!A59,Sheet1!A59,"")</f>
         <v>15</v>
@@ -9861,7 +9873,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <f>IF(Sheet1!A60=Sheet2!A60,Sheet1!A60,"")</f>
         <v>15</v>
@@ -9887,7 +9899,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <f>IF(Sheet1!A61=Sheet2!A61,Sheet1!A61,"")</f>
         <v>15</v>
@@ -9913,7 +9925,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <f>IF(Sheet1!A62=Sheet2!A62,Sheet1!A62,"")</f>
         <v>15</v>
@@ -9939,7 +9951,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <f>IF(Sheet1!A63=Sheet2!A63,Sheet1!A63,"")</f>
         <v>16</v>
@@ -9965,7 +9977,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <f>IF(Sheet1!A64=Sheet2!A64,Sheet1!A64,"")</f>
         <v>16</v>
@@ -9991,7 +10003,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <f>IF(Sheet1!A65=Sheet2!A65,Sheet1!A65,"")</f>
         <v>16</v>
@@ -10017,7 +10029,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <f>IF(Sheet1!A66=Sheet2!A66,Sheet1!A66,"")</f>
         <v>16</v>
@@ -10043,7 +10055,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <f>IF(Sheet1!A67=Sheet2!A67,Sheet1!A67,"")</f>
         <v>17</v>
@@ -10069,7 +10081,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <f>IF(Sheet1!A68=Sheet2!A68,Sheet1!A68,"")</f>
         <v>17</v>
@@ -10095,7 +10107,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <f>IF(Sheet1!A69=Sheet2!A69,Sheet1!A69,"")</f>
         <v>17</v>
@@ -10121,7 +10133,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <f>IF(Sheet1!A70=Sheet2!A70,Sheet1!A70,"")</f>
         <v>17</v>
@@ -10147,7 +10159,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <f>IF(Sheet1!A71=Sheet2!A71,Sheet1!A71,"")</f>
         <v>18</v>
@@ -10173,7 +10185,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <f>IF(Sheet1!A72=Sheet2!A72,Sheet1!A72,"")</f>
         <v>18</v>
@@ -10199,7 +10211,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <f>IF(Sheet1!A73=Sheet2!A73,Sheet1!A73,"")</f>
         <v>18</v>
@@ -10225,7 +10237,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <f>IF(Sheet1!A74=Sheet2!A74,Sheet1!A74,"")</f>
         <v>18</v>
@@ -10251,7 +10263,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <f>IF(Sheet1!A75=Sheet2!A75,Sheet1!A75,"")</f>
         <v>19</v>
@@ -10277,7 +10289,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <f>IF(Sheet1!A76=Sheet2!A76,Sheet1!A76,"")</f>
         <v>19</v>
@@ -10303,7 +10315,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <f>IF(Sheet1!A77=Sheet2!A77,Sheet1!A77,"")</f>
         <v>19</v>
@@ -10329,7 +10341,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <f>IF(Sheet1!A78=Sheet2!A78,Sheet1!A78,"")</f>
         <v>19</v>
@@ -10355,7 +10367,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <f>IF(Sheet1!A79=Sheet2!A79,Sheet1!A79,"")</f>
         <v>20</v>
@@ -10381,7 +10393,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <f>IF(Sheet1!A80=Sheet2!A80,Sheet1!A80,"")</f>
         <v>20</v>
@@ -10407,7 +10419,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <f>IF(Sheet1!A81=Sheet2!A81,Sheet1!A81,"")</f>
         <v>20</v>
@@ -10418,7 +10430,7 @@
       </c>
       <c r="C81" t="str">
         <f>IF(Sheet1!C81=Sheet2!C81,Sheet1!C81,"")</f>
-        <v>cob</v>
+        <v/>
       </c>
       <c r="D81" t="str">
         <f>IF(Sheet1!D81=Sheet2!D81,Sheet1!D81,"")</f>
@@ -10433,7 +10445,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <f>IF(Sheet1!A82=Sheet2!A82,Sheet1!A82,"")</f>
         <v>20</v>
@@ -10444,7 +10456,7 @@
       </c>
       <c r="C82" t="str">
         <f>IF(Sheet1!C82=Sheet2!C82,Sheet1!C82,"")</f>
-        <v>coz</v>
+        <v/>
       </c>
       <c r="D82" t="str">
         <f>IF(Sheet1!D82=Sheet2!D82,Sheet1!D82,"")</f>
@@ -10459,7 +10471,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <f>IF(Sheet1!A83=Sheet2!A83,Sheet1!A83,"")</f>
         <v>21</v>
@@ -10485,7 +10497,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <f>IF(Sheet1!A84=Sheet2!A84,Sheet1!A84,"")</f>
         <v>21</v>
@@ -10511,7 +10523,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <f>IF(Sheet1!A85=Sheet2!A85,Sheet1!A85,"")</f>
         <v>21</v>
@@ -10537,7 +10549,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <f>IF(Sheet1!A86=Sheet2!A86,Sheet1!A86,"")</f>
         <v>21</v>
@@ -10563,7 +10575,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <f>IF(Sheet1!A87=Sheet2!A87,Sheet1!A87,"")</f>
         <v>22</v>
@@ -10589,7 +10601,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <f>IF(Sheet1!A88=Sheet2!A88,Sheet1!A88,"")</f>
         <v>22</v>
@@ -10615,7 +10627,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <f>IF(Sheet1!A89=Sheet2!A89,Sheet1!A89,"")</f>
         <v>22</v>
@@ -10641,7 +10653,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <f>IF(Sheet1!A90=Sheet2!A90,Sheet1!A90,"")</f>
         <v>22</v>
@@ -10667,7 +10679,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <f>IF(Sheet1!A91=Sheet2!A91,Sheet1!A91,"")</f>
         <v>23</v>
@@ -10693,7 +10705,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <f>IF(Sheet1!A92=Sheet2!A92,Sheet1!A92,"")</f>
         <v>23</v>
@@ -10719,7 +10731,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <f>IF(Sheet1!A93=Sheet2!A93,Sheet1!A93,"")</f>
         <v>23</v>
@@ -10745,7 +10757,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <f>IF(Sheet1!A94=Sheet2!A94,Sheet1!A94,"")</f>
         <v>23</v>
@@ -10771,7 +10783,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <f>IF(Sheet1!A95=Sheet2!A95,Sheet1!A95,"")</f>
         <v>24</v>
@@ -10797,7 +10809,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <f>IF(Sheet1!A96=Sheet2!A96,Sheet1!A96,"")</f>
         <v>24</v>
@@ -10823,7 +10835,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <f>IF(Sheet1!A97=Sheet2!A97,Sheet1!A97,"")</f>
         <v>24</v>
@@ -10849,7 +10861,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <f>IF(Sheet1!A98=Sheet2!A98,Sheet1!A98,"")</f>
         <v>24</v>
@@ -10875,7 +10887,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <f>IF(Sheet1!A99=Sheet2!A99,Sheet1!A99,"")</f>
         <v>25</v>
@@ -10901,7 +10913,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <f>IF(Sheet1!A100=Sheet2!A100,Sheet1!A100,"")</f>
         <v>25</v>
@@ -10927,7 +10939,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <f>IF(Sheet1!A101=Sheet2!A101,Sheet1!A101,"")</f>
         <v>25</v>
@@ -10953,7 +10965,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <f>IF(Sheet1!A102=Sheet2!A102,Sheet1!A102,"")</f>
         <v>25</v>
@@ -10979,7 +10991,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <f>IF(Sheet1!A103=Sheet2!A103,Sheet1!A103,"")</f>
         <v>26</v>
@@ -11005,7 +11017,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <f>IF(Sheet1!A104=Sheet2!A104,Sheet1!A104,"")</f>
         <v>26</v>
@@ -11031,7 +11043,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <f>IF(Sheet1!A105=Sheet2!A105,Sheet1!A105,"")</f>
         <v>26</v>
@@ -11057,7 +11069,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <f>IF(Sheet1!A106=Sheet2!A106,Sheet1!A106,"")</f>
         <v>26</v>
@@ -11083,7 +11095,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <f>IF(Sheet1!A107=Sheet2!A107,Sheet1!A107,"")</f>
         <v>27</v>
@@ -11109,7 +11121,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <f>IF(Sheet1!A108=Sheet2!A108,Sheet1!A108,"")</f>
         <v>27</v>
@@ -11135,7 +11147,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <f>IF(Sheet1!A109=Sheet2!A109,Sheet1!A109,"")</f>
         <v>27</v>
@@ -11161,7 +11173,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <f>IF(Sheet1!A110=Sheet2!A110,Sheet1!A110,"")</f>
         <v>27</v>
@@ -11187,7 +11199,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <f>IF(Sheet1!A111=Sheet2!A111,Sheet1!A111,"")</f>
         <v>28</v>
@@ -11213,7 +11225,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <f>IF(Sheet1!A112=Sheet2!A112,Sheet1!A112,"")</f>
         <v>28</v>
@@ -11239,7 +11251,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <f>IF(Sheet1!A113=Sheet2!A113,Sheet1!A113,"")</f>
         <v>28</v>
@@ -11265,7 +11277,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <f>IF(Sheet1!A114=Sheet2!A114,Sheet1!A114,"")</f>
         <v>28</v>
@@ -11291,7 +11303,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <f>IF(Sheet1!A115=Sheet2!A115,Sheet1!A115,"")</f>
         <v>29</v>
@@ -11317,7 +11329,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <f>IF(Sheet1!A116=Sheet2!A116,Sheet1!A116,"")</f>
         <v>29</v>
@@ -11343,7 +11355,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <f>IF(Sheet1!A117=Sheet2!A117,Sheet1!A117,"")</f>
         <v>29</v>
@@ -11369,7 +11381,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <f>IF(Sheet1!A118=Sheet2!A118,Sheet1!A118,"")</f>
         <v>29</v>
@@ -11395,7 +11407,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <f>IF(Sheet1!A119=Sheet2!A119,Sheet1!A119,"")</f>
         <v>30</v>
@@ -11421,7 +11433,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <f>IF(Sheet1!A120=Sheet2!A120,Sheet1!A120,"")</f>
         <v>30</v>
@@ -11447,7 +11459,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <f>IF(Sheet1!A121=Sheet2!A121,Sheet1!A121,"")</f>
         <v>30</v>
@@ -11473,7 +11485,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <f>IF(Sheet1!A122=Sheet2!A122,Sheet1!A122,"")</f>
         <v>30</v>
@@ -11499,7 +11511,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <f>IF(Sheet1!A123=Sheet2!A123,Sheet1!A123,"")</f>
         <v>31</v>
@@ -11525,7 +11537,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <f>IF(Sheet1!A124=Sheet2!A124,Sheet1!A124,"")</f>
         <v>31</v>
@@ -11551,7 +11563,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <f>IF(Sheet1!A125=Sheet2!A125,Sheet1!A125,"")</f>
         <v>31</v>
@@ -11577,7 +11589,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <f>IF(Sheet1!A126=Sheet2!A126,Sheet1!A126,"")</f>
         <v>31</v>
@@ -11603,7 +11615,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <f>IF(Sheet1!A127=Sheet2!A127,Sheet1!A127,"")</f>
         <v>32</v>
@@ -11629,7 +11641,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <f>IF(Sheet1!A128=Sheet2!A128,Sheet1!A128,"")</f>
         <v>32</v>
@@ -11655,7 +11667,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <f>IF(Sheet1!A129=Sheet2!A129,Sheet1!A129,"")</f>
         <v>32</v>
@@ -11681,7 +11693,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <f>IF(Sheet1!A130=Sheet2!A130,Sheet1!A130,"")</f>
         <v>32</v>
@@ -11707,7 +11719,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <f>IF(Sheet1!A131=Sheet2!A131,Sheet1!A131,"")</f>
         <v>33</v>
@@ -11733,7 +11745,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <f>IF(Sheet1!A132=Sheet2!A132,Sheet1!A132,"")</f>
         <v>33</v>
@@ -11759,7 +11771,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <f>IF(Sheet1!A133=Sheet2!A133,Sheet1!A133,"")</f>
         <v>33</v>
@@ -11785,7 +11797,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <f>IF(Sheet1!A134=Sheet2!A134,Sheet1!A134,"")</f>
         <v>33</v>
@@ -11811,7 +11823,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <f>IF(Sheet1!A135=Sheet2!A135,Sheet1!A135,"")</f>
         <v>34</v>
@@ -11837,7 +11849,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <f>IF(Sheet1!A136=Sheet2!A136,Sheet1!A136,"")</f>
         <v>34</v>
@@ -11863,7 +11875,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <f>IF(Sheet1!A137=Sheet2!A137,Sheet1!A137,"")</f>
         <v>34</v>
@@ -11889,7 +11901,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <f>IF(Sheet1!A138=Sheet2!A138,Sheet1!A138,"")</f>
         <v>34</v>
@@ -11915,7 +11927,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <f>IF(Sheet1!A139=Sheet2!A139,Sheet1!A139,"")</f>
         <v>35</v>
@@ -11941,7 +11953,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <f>IF(Sheet1!A140=Sheet2!A140,Sheet1!A140,"")</f>
         <v>35</v>
@@ -11967,7 +11979,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <f>IF(Sheet1!A141=Sheet2!A141,Sheet1!A141,"")</f>
         <v>35</v>
@@ -11993,7 +12005,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <f>IF(Sheet1!A142=Sheet2!A142,Sheet1!A142,"")</f>
         <v>35</v>
@@ -12019,7 +12031,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <f>IF(Sheet1!A143=Sheet2!A143,Sheet1!A143,"")</f>
         <v>36</v>
@@ -12045,7 +12057,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <f>IF(Sheet1!A144=Sheet2!A144,Sheet1!A144,"")</f>
         <v>36</v>
@@ -12071,7 +12083,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <f>IF(Sheet1!A145=Sheet2!A145,Sheet1!A145,"")</f>
         <v>36</v>
@@ -12097,7 +12109,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <f>IF(Sheet1!A146=Sheet2!A146,Sheet1!A146,"")</f>
         <v>36</v>
@@ -12123,7 +12135,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <f>IF(Sheet1!A147=Sheet2!A147,Sheet1!A147,"")</f>
         <v>37</v>
@@ -12149,7 +12161,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <f>IF(Sheet1!A148=Sheet2!A148,Sheet1!A148,"")</f>
         <v>37</v>
@@ -12175,7 +12187,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <f>IF(Sheet1!A149=Sheet2!A149,Sheet1!A149,"")</f>
         <v>37</v>
@@ -12201,7 +12213,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <f>IF(Sheet1!A150=Sheet2!A150,Sheet1!A150,"")</f>
         <v>37</v>
@@ -12227,7 +12239,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <f>IF(Sheet1!A151=Sheet2!A151,Sheet1!A151,"")</f>
         <v>38</v>
@@ -12253,7 +12265,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <f>IF(Sheet1!A152=Sheet2!A152,Sheet1!A152,"")</f>
         <v>38</v>
@@ -12279,7 +12291,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <f>IF(Sheet1!A153=Sheet2!A153,Sheet1!A153,"")</f>
         <v>38</v>
@@ -12305,7 +12317,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <f>IF(Sheet1!A154=Sheet2!A154,Sheet1!A154,"")</f>
         <v>38</v>
@@ -12331,7 +12343,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <f>IF(Sheet1!A155=Sheet2!A155,Sheet1!A155,"")</f>
         <v>39</v>
@@ -12357,7 +12369,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <f>IF(Sheet1!A156=Sheet2!A156,Sheet1!A156,"")</f>
         <v>39</v>
@@ -12383,7 +12395,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <f>IF(Sheet1!A157=Sheet2!A157,Sheet1!A157,"")</f>
         <v>39</v>
@@ -12409,7 +12421,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <f>IF(Sheet1!A158=Sheet2!A158,Sheet1!A158,"")</f>
         <v>39</v>
@@ -12435,7 +12447,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <f>IF(Sheet1!A159=Sheet2!A159,Sheet1!A159,"")</f>
         <v>40</v>
@@ -12461,7 +12473,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <f>IF(Sheet1!A160=Sheet2!A160,Sheet1!A160,"")</f>
         <v>40</v>
@@ -12487,7 +12499,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <f>IF(Sheet1!A161=Sheet2!A161,Sheet1!A161,"")</f>
         <v>40</v>
@@ -12513,7 +12525,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <f>IF(Sheet1!A162=Sheet2!A162,Sheet1!A162,"")</f>
         <v>40</v>
@@ -12539,7 +12551,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <f>IF(Sheet1!A163=Sheet2!A163,Sheet1!A163,"")</f>
         <v>41</v>
@@ -12565,7 +12577,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <f>IF(Sheet1!A164=Sheet2!A164,Sheet1!A164,"")</f>
         <v>41</v>
@@ -12591,7 +12603,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <f>IF(Sheet1!A165=Sheet2!A165,Sheet1!A165,"")</f>
         <v>41</v>
@@ -12617,7 +12629,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <f>IF(Sheet1!A166=Sheet2!A166,Sheet1!A166,"")</f>
         <v>41</v>
@@ -12643,7 +12655,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <f>IF(Sheet1!A167=Sheet2!A167,Sheet1!A167,"")</f>
         <v>42</v>
@@ -12669,7 +12681,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <f>IF(Sheet1!A168=Sheet2!A168,Sheet1!A168,"")</f>
         <v>42</v>
@@ -12695,7 +12707,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <f>IF(Sheet1!A169=Sheet2!A169,Sheet1!A169,"")</f>
         <v>42</v>
@@ -12721,7 +12733,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <f>IF(Sheet1!A170=Sheet2!A170,Sheet1!A170,"")</f>
         <v>42</v>
@@ -12747,7 +12759,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <f>IF(Sheet1!A171=Sheet2!A171,Sheet1!A171,"")</f>
         <v>43</v>
@@ -12773,7 +12785,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <f>IF(Sheet1!A172=Sheet2!A172,Sheet1!A172,"")</f>
         <v>43</v>
@@ -12799,7 +12811,7 @@
         <v>E</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <f>IF(Sheet1!A173=Sheet2!A173,Sheet1!A173,"")</f>
         <v>43</v>
@@ -12825,7 +12837,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <f>IF(Sheet1!A174=Sheet2!A174,Sheet1!A174,"")</f>
         <v>43</v>

</xml_diff>